<commit_message>
Update CTBSCAN + fast log integrale CTB250
</commit_message>
<xml_diff>
--- a/Docs/ActiveCTB.xlsx
+++ b/Docs/ActiveCTB.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="201">
   <si>
     <t>ID. M-Bus</t>
   </si>
@@ -542,9 +542,6 @@
     <t>00000117</t>
   </si>
   <si>
-    <t>00000118??</t>
-  </si>
-  <si>
     <t>00000120</t>
   </si>
   <si>
@@ -620,17 +617,23 @@
     <t>Cond. Banca e Supermarket - LOTTO 8</t>
   </si>
   <si>
-    <t>Condomini V A R I - STC  53</t>
-  </si>
-  <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>GUASTO</t>
+  </si>
+  <si>
+    <t>00000118</t>
+  </si>
+  <si>
+    <t>Condominio 53</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,8 +656,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -678,8 +703,18 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -702,12 +737,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -733,16 +785,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Valore non valido" xfId="1" builtinId="27"/>
+    <cellStyle name="Valore valido" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1020,11 +1080,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H123"/>
+  <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1100,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1065,25 +1125,34 @@
       <c r="H1" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>119</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>19</v>
       </c>
@@ -1107,7 +1176,7 @@
       </c>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -1118,7 +1187,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -1131,7 +1200,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -1148,7 +1217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>26</v>
       </c>
@@ -1165,7 +1234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>27</v>
       </c>
@@ -1188,10 +1257,10 @@
         <v>8</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>35</v>
       </c>
@@ -1217,7 +1286,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>36</v>
       </c>
@@ -1243,7 +1312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>38</v>
       </c>
@@ -1265,9 +1334,11 @@
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>39</v>
       </c>
@@ -1281,7 +1352,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>40</v>
       </c>
@@ -1305,7 +1376,7 @@
       </c>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>41</v>
       </c>
@@ -1331,7 +1402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42</v>
       </c>
@@ -1355,7 +1426,7 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45</v>
       </c>
@@ -1381,7 +1452,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>46</v>
       </c>
@@ -1504,11 +1575,20 @@
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F21" s="3" t="s">
         <v>123</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>18</v>
@@ -1698,7 +1778,7 @@
         <v>44</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>
@@ -1709,7 +1789,9 @@
       <c r="G29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="6"/>
+      <c r="H29" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -1733,7 +1815,9 @@
       <c r="G30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="H30" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -1757,7 +1841,9 @@
       <c r="G31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="6"/>
+      <c r="H31" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -1781,7 +1867,9 @@
       <c r="G32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="6"/>
+      <c r="H32" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -1828,6 +1916,9 @@
       <c r="G34" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -1926,8 +2017,11 @@
       <c r="F38" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>8</v>
+      <c r="G38" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1952,7 +2046,9 @@
       <c r="G39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H39" s="6"/>
+      <c r="H39" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
@@ -1976,6 +2072,9 @@
       <c r="G40" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="H40" s="11" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
@@ -1999,7 +2098,9 @@
       <c r="G41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H41" s="6"/>
+      <c r="H41" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -2023,7 +2124,9 @@
       <c r="G42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="6"/>
+      <c r="H42" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -2047,7 +2150,9 @@
       <c r="G43" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H43" s="6"/>
+      <c r="H43" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
@@ -2071,7 +2176,9 @@
       <c r="G44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H44" s="6"/>
+      <c r="H44" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
@@ -2457,7 +2564,9 @@
       <c r="G59" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H59" s="6"/>
+      <c r="H59" s="7" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
@@ -2481,7 +2590,9 @@
       <c r="G60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H60" s="6"/>
+      <c r="H60" s="7" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
@@ -2525,71 +2636,71 @@
       <c r="E62" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F62" s="9" t="s">
-        <v>172</v>
+      <c r="F62" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H62" s="10" t="s">
+      <c r="H62" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>198</v>
+        <v>40</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H63" s="10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>39</v>
+      <c r="C64" s="1">
+        <v>13</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="1">
-        <v>13</v>
+      <c r="C65" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>36</v>
@@ -2600,22 +2711,20 @@
       <c r="G65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H65" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="H65" s="6"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>36</v>
@@ -2626,20 +2735,22 @@
       <c r="G66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="6"/>
+      <c r="H66" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>36</v>
@@ -2650,25 +2761,23 @@
       <c r="G67" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H67" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="H67" s="6"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>176</v>
@@ -2680,19 +2789,19 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>177</v>
@@ -2704,16 +2813,16 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>36</v>
@@ -2728,16 +2837,16 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>36</v>
@@ -2752,40 +2861,33 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H72" s="6"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>36</v>
@@ -2793,33 +2895,42 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>36</v>
@@ -2834,16 +2945,16 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>36</v>
@@ -2854,20 +2965,22 @@
       <c r="G76" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H76" s="6"/>
+      <c r="H76" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>36</v>
@@ -2882,19 +2995,19 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>184</v>
@@ -2902,20 +3015,22 @@
       <c r="G78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H78" s="6"/>
+      <c r="H78" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>67</v>
+      <c r="C79" s="1">
+        <v>12</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>14</v>
@@ -2932,19 +3047,19 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C80" s="1">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>186</v>
@@ -2958,19 +3073,19 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C81" s="1">
-        <v>25</v>
+      <c r="C81" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>187</v>
@@ -2978,87 +3093,78 @@
       <c r="G81" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H81" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="H81" s="6"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H82" s="6"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H83" s="6"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H84" s="6"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>7</v>
@@ -3066,50 +3172,59 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F87" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H87" s="11" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>190</v>
@@ -3117,22 +3232,25 @@
       <c r="G88" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="H88" s="7" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>191</v>
@@ -3140,23 +3258,25 @@
       <c r="G89" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H89" s="6"/>
+      <c r="H89" s="11" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>192</v>
@@ -3164,30 +3284,23 @@
       <c r="G90" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="H90" s="7" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>192</v>
+      <c r="A91" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H91" s="6"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
@@ -3197,10 +3310,10 @@
         <v>22</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3211,7 +3324,7 @@
         <v>22</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>24</v>
@@ -3222,30 +3335,30 @@
         <v>80</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3256,7 +3369,7 @@
         <v>22</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>24</v>
@@ -3270,7 +3383,7 @@
         <v>22</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>24</v>
@@ -3284,7 +3397,7 @@
         <v>22</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>24</v>
@@ -3298,7 +3411,7 @@
         <v>22</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>24</v>
@@ -3312,7 +3425,7 @@
         <v>22</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>24</v>
@@ -3326,7 +3439,7 @@
         <v>22</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>24</v>
@@ -3340,7 +3453,7 @@
         <v>22</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>24</v>
@@ -3354,7 +3467,7 @@
         <v>22</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>24</v>
@@ -3368,7 +3481,7 @@
         <v>22</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>24</v>
@@ -3382,10 +3495,10 @@
         <v>22</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3396,10 +3509,10 @@
         <v>22</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3410,7 +3523,7 @@
         <v>22</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>99</v>
@@ -3424,7 +3537,7 @@
         <v>22</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>99</v>
@@ -3441,7 +3554,7 @@
         <v>101</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3452,7 +3565,7 @@
         <v>22</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>24</v>
@@ -3469,7 +3582,7 @@
         <v>102</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3480,10 +3593,10 @@
         <v>22</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3497,7 +3610,7 @@
         <v>103</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3508,24 +3621,24 @@
         <v>22</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3536,7 +3649,7 @@
         <v>22</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>99</v>
@@ -3550,10 +3663,10 @@
         <v>22</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3564,7 +3677,7 @@
         <v>22</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>109</v>
@@ -3578,10 +3691,10 @@
         <v>22</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3592,7 +3705,7 @@
         <v>22</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>99</v>
@@ -3606,7 +3719,7 @@
         <v>22</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>99</v>
@@ -3620,27 +3733,14 @@
         <v>22</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>